<commit_message>
Correzione Files Eliot CS per errato test 191
Correzione Files Eliot CS per errato test 191
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Eliot_CS/20.16.00/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Eliot_CS/20.16.00/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\DOCUMENTI\CDA_FSE2.0\AccreditamentoFSE20\Eliot_CS\20.16.00\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B05CCFF-E17B-4D84-B199-E13B4C6B46F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F198A6-798D-4D93-BD26-1457603D67AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -765,15 +765,6 @@
     <t>7e0fc50c9b7b1164</t>
   </si>
   <si>
-    <t>2023-03-21T10:00:45Z</t>
-  </si>
-  <si>
-    <t>89a282ccedf9253d</t>
-  </si>
-  <si>
-    <t>"2.16.840.1.113883.2.9.2.150.4.4.bf7a4d5266cc2c2d9ccab8ae8868d281c206dcf4aeb3c6d7ea6ce68bfd4078d1.c9bd08eebf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
-  </si>
-  <si>
     <t>Errore di collegamento al Gateway</t>
   </si>
   <si>
@@ -832,6 +823,15 @@
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Il Documento CDA2 Laboratorio dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 5" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
 </t>
+  </si>
+  <si>
+    <t>2023-04-06T16:46:53Z</t>
+  </si>
+  <si>
+    <t>bf52b5a2ef817c6f</t>
+  </si>
+  <si>
+    <t>"2.16.840.1.113883.2.9.2.150.4.4.46fdef890a0196744ed983281313dde2494d214b1d1c022420c71c4324c0ce27.5e4477e689^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
   </si>
 </sst>
 </file>
@@ -1289,28 +1289,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1340,6 +1318,28 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2787,10 +2787,10 @@
   <dimension ref="A1:T823"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2830,14 +2830,14 @@
       <c r="T1" s="32"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="39" t="s">
+      <c r="B2" s="48"/>
+      <c r="C2" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="38"/>
+      <c r="D2" s="48"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -2855,14 +2855,14 @@
       <c r="T2" s="32"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="46" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="38"/>
+      <c r="D3" s="48"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -2880,12 +2880,12 @@
       <c r="T3" s="32"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="46" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="2"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -2904,12 +2904,12 @@
       <c r="T4" s="32"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="46" t="s">
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="48"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -2927,8 +2927,8 @@
       <c r="T5" s="32"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -3046,35 +3046,35 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="47">
+      <c r="A10" s="35">
         <v>1</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="E10" s="49" t="s">
-        <v>173</v>
-      </c>
-      <c r="F10" s="50"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="52" t="s">
+      <c r="D10" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10" s="38"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="K10" s="52" t="s">
-        <v>174</v>
-      </c>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="54"/>
+      <c r="K10" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="42"/>
       <c r="P10" s="19"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="21"/>
@@ -3082,35 +3082,35 @@
       <c r="T10" s="19"/>
     </row>
     <row r="11" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="47">
+      <c r="A11" s="35">
         <v>2</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="E11" s="49" t="s">
-        <v>176</v>
-      </c>
-      <c r="F11" s="50"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="52" t="s">
+      <c r="D11" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="K11" s="55" t="s">
-        <v>174</v>
-      </c>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="54"/>
+      <c r="K11" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="42"/>
       <c r="P11" s="19"/>
       <c r="Q11" s="20"/>
       <c r="R11" s="21"/>
@@ -3118,35 +3118,35 @@
       <c r="T11" s="19"/>
     </row>
     <row r="12" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="47">
+      <c r="A12" s="35">
         <v>3</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="E12" s="49" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12" s="50"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="52" t="s">
+      <c r="D12" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" s="38"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="K12" s="52" t="s">
-        <v>174</v>
-      </c>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="54"/>
+      <c r="K12" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="42"/>
       <c r="P12" s="19"/>
       <c r="Q12" s="20"/>
       <c r="R12" s="21"/>
@@ -3154,35 +3154,35 @@
       <c r="T12" s="19"/>
     </row>
     <row r="13" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47">
+      <c r="A13" s="35">
         <v>4</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="E13" s="49" t="s">
-        <v>180</v>
-      </c>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="56" t="s">
+      <c r="D13" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13" s="38"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="K13" s="52" t="s">
-        <v>174</v>
-      </c>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="54"/>
+      <c r="K13" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="42"/>
       <c r="P13" s="19"/>
       <c r="Q13" s="20"/>
       <c r="R13" s="21"/>
@@ -3190,35 +3190,35 @@
       <c r="T13" s="19"/>
     </row>
     <row r="14" spans="1:20" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47">
+      <c r="A14" s="35">
         <v>5</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="E14" s="49" t="s">
-        <v>182</v>
-      </c>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52" t="s">
+      <c r="D14" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="K14" s="52" t="s">
-        <v>174</v>
-      </c>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="53"/>
-      <c r="O14" s="54"/>
+      <c r="K14" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="42"/>
       <c r="P14" s="19"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="21"/>
@@ -3264,7 +3264,7 @@
         <v>33</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O15" s="19" t="s">
         <v>33</v>
@@ -3318,7 +3318,7 @@
         <v>33</v>
       </c>
       <c r="N16" s="19" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O16" s="19" t="s">
         <v>33</v>
@@ -3414,7 +3414,7 @@
         <v>33</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="O18" s="19" t="s">
         <v>33</v>
@@ -3453,7 +3453,7 @@
         <v>76</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
@@ -3506,7 +3506,7 @@
         <v>33</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="O20" s="19" t="s">
         <v>33</v>
@@ -3970,16 +3970,16 @@
         <v>84</v>
       </c>
       <c r="F29" s="17">
-        <v>45006</v>
+        <v>45022</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>33</v>
@@ -19967,6 +19967,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
@@ -19975,15 +19984,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20006,6 +20006,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
@@ -20022,14 +20030,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Rieseguiti i test 28 e 36
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Eliot_CS/20.16.00/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Eliot_CS/20.16.00/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\DOCUMENTI\CDA_FSE2.0\AccreditamentoFSE20\Eliot_CS\20.16.00\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F198A6-798D-4D93-BD26-1457603D67AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE8A083-89CC-4ECA-A1EE-7FDC2E370EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -657,19 +657,7 @@
     <t>subject_application_version:20.16.00</t>
   </si>
   <si>
-    <t>2023-03-21T10:25:42Z</t>
-  </si>
-  <si>
-    <t>fff059526fd10336</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
-  </si>
-  <si>
-    <t>2013-03-21T10:29:13Z</t>
-  </si>
-  <si>
-    <t>38c2fadba961a75c</t>
   </si>
   <si>
     <t>2023-03-21T10:33:00Z</t>
@@ -832,6 +820,18 @@
   </si>
   <si>
     <t>"2.16.840.1.113883.2.9.2.150.4.4.46fdef890a0196744ed983281313dde2494d214b1d1c022420c71c4324c0ce27.5e4477e689^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"</t>
+  </si>
+  <si>
+    <t>2023-04-26T12:18:53Z</t>
+  </si>
+  <si>
+    <t>8bcc606934faab83</t>
+  </si>
+  <si>
+    <t>1c1939e64c0ddd0f</t>
+  </si>
+  <si>
+    <t>2023-04-26T12:24:02Z</t>
   </si>
 </sst>
 </file>
@@ -2787,10 +2787,10 @@
   <dimension ref="A1:T823"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3056,10 +3056,10 @@
         <v>26</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F10" s="38"/>
       <c r="G10" s="39"/>
@@ -3069,7 +3069,7 @@
         <v>76</v>
       </c>
       <c r="K10" s="40" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="L10" s="40"/>
       <c r="M10" s="40"/>
@@ -3092,10 +3092,10 @@
         <v>26</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F11" s="38"/>
       <c r="G11" s="39"/>
@@ -3105,7 +3105,7 @@
         <v>76</v>
       </c>
       <c r="K11" s="43" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="L11" s="40"/>
       <c r="M11" s="40"/>
@@ -3128,10 +3128,10 @@
         <v>26</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F12" s="38"/>
       <c r="G12" s="39"/>
@@ -3141,7 +3141,7 @@
         <v>76</v>
       </c>
       <c r="K12" s="40" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="L12" s="40"/>
       <c r="M12" s="40"/>
@@ -3164,10 +3164,10 @@
         <v>26</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F13" s="38"/>
       <c r="G13" s="39"/>
@@ -3177,7 +3177,7 @@
         <v>76</v>
       </c>
       <c r="K13" s="40" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="L13" s="40"/>
       <c r="M13" s="40"/>
@@ -3200,10 +3200,10 @@
         <v>26</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F14" s="38"/>
       <c r="G14" s="39"/>
@@ -3213,7 +3213,7 @@
         <v>76</v>
       </c>
       <c r="K14" s="40" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="L14" s="40"/>
       <c r="M14" s="40"/>
@@ -3242,16 +3242,16 @@
         <v>104</v>
       </c>
       <c r="F15" s="17">
-        <v>45006</v>
+        <v>45042</v>
       </c>
       <c r="G15" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="I15" s="18" t="s">
         <v>129</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>131</v>
       </c>
       <c r="J15" s="19" t="s">
         <v>33</v>
@@ -3264,7 +3264,7 @@
         <v>33</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="O15" s="19" t="s">
         <v>33</v>
@@ -3296,16 +3296,16 @@
         <v>105</v>
       </c>
       <c r="F16" s="17">
-        <v>45006</v>
+        <v>45042</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>133</v>
+        <v>180</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J16" s="19" t="s">
         <v>33</v>
@@ -3318,7 +3318,7 @@
         <v>33</v>
       </c>
       <c r="N16" s="19" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="O16" s="19" t="s">
         <v>33</v>
@@ -3353,7 +3353,7 @@
         <v>45006</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -3395,13 +3395,13 @@
         <v>45006</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J18" s="19" t="s">
         <v>33</v>
@@ -3414,7 +3414,7 @@
         <v>33</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="O18" s="19" t="s">
         <v>33</v>
@@ -3453,7 +3453,7 @@
         <v>76</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
@@ -3487,13 +3487,13 @@
         <v>45006</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>33</v>
@@ -3506,7 +3506,7 @@
         <v>33</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="O20" s="19" t="s">
         <v>33</v>
@@ -3541,13 +3541,13 @@
         <v>45006</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J21" s="19" t="s">
         <v>33</v>
@@ -3595,13 +3595,13 @@
         <v>45006</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J22" s="19" t="s">
         <v>33</v>
@@ -3649,13 +3649,13 @@
         <v>45006</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>33</v>
@@ -3703,13 +3703,13 @@
         <v>45006</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J24" s="19" t="s">
         <v>33</v>
@@ -3757,13 +3757,13 @@
         <v>45006</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J25" s="19" t="s">
         <v>33</v>
@@ -3811,13 +3811,13 @@
         <v>45007</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J26" s="19" t="s">
         <v>33</v>
@@ -3865,13 +3865,13 @@
         <v>45007</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>33</v>
@@ -3919,13 +3919,13 @@
         <v>45007</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J28" s="19" t="s">
         <v>33</v>
@@ -3973,13 +3973,13 @@
         <v>45022</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>33</v>
@@ -19967,15 +19967,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
@@ -19984,6 +19975,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20006,14 +20006,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1940EA21-F316-4004-B0A9-40138AAC7DA1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
@@ -20030,6 +20022,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D58B9263-706C-436D-BB9D-8B538C07064D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>